<commit_message>
upd xlsx for lab 27
</commit_message>
<xml_diff>
--- a/lab27/ФИСТ2023_ЛР27_Время_работы_разных_реализаций_Словаря.xlsx
+++ b/lab27/ФИСТ2023_ЛР27_Время_работы_разных_реализаций_Словаря.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studying ULSTU\1 курс\ОАиП\Мои Лабы\lab27\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5377665F-E799-4B2A-AB70-F67D8EC7E528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E6900C-8B80-401B-839C-47F145DCCED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="СВОДНАЯ" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="37">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -128,6 +128,15 @@
   </si>
   <si>
     <t>#define MAX_HASH 1</t>
+  </si>
+  <si>
+    <t>Очень много простой, но рутинной работы</t>
+  </si>
+  <si>
+    <t>Сущенствует много способов решения одной задачи</t>
+  </si>
+  <si>
+    <t>Хэш таблицы быстрее:)</t>
   </si>
 </sst>
 </file>
@@ -188,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -197,6 +206,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -539,7 +551,7 @@
   <dimension ref="B1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,19 +645,28 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C22" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="C26" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>